<commit_message>
Updates to the game. The game now functions but still without the functions of the speech recognizer and inclusion of test sentences.
</commit_message>
<xml_diff>
--- a/src/Game/map.xlsx
+++ b/src/Game/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20180" yWindow="8040" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="9600" yWindow="2920" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>StartingRoom</t>
   </si>
@@ -32,10 +32,16 @@
     <t>EmptyWoodsPath</t>
   </si>
   <si>
-    <t>EnemyRoom</t>
-  </si>
-  <si>
-    <t>LeaveCaveRoom</t>
+    <t>ExitRoom</t>
+  </si>
+  <si>
+    <t>EvilTwinsRoom</t>
+  </si>
+  <si>
+    <t>PPRoom</t>
+  </si>
+  <si>
+    <t>BossRoom</t>
   </si>
 </sst>
 </file>
@@ -353,7 +359,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -367,23 +373,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -391,18 +403,18 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -416,27 +428,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>

</xml_diff>